<commit_message>
dodane upute za neke od zahtjeva
</commit_message>
<xml_diff>
--- a/pesi.xlsx
+++ b/pesi.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="42220" yWindow="4760" windowWidth="25600" windowHeight="15120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="132">
   <si>
     <t>Energy level</t>
   </si>
@@ -33,33 +33,6 @@
     <t>Affection level</t>
   </si>
   <si>
-    <t>Friendliness toward other dogs</t>
-  </si>
-  <si>
-    <t>Friendliness toward other pets</t>
-  </si>
-  <si>
-    <t>Friendliness toward strangers</t>
-  </si>
-  <si>
-    <t>Ease of training</t>
-  </si>
-  <si>
-    <t>Watchdog ability</t>
-  </si>
-  <si>
-    <t>Protection ability</t>
-  </si>
-  <si>
-    <t>Grooming needs</t>
-  </si>
-  <si>
-    <t>Cold tolerance</t>
-  </si>
-  <si>
-    <t>Heat tolerance</t>
-  </si>
-  <si>
     <t>Australian Cattle Dog</t>
   </si>
   <si>
@@ -415,6 +388,33 @@
   </si>
   <si>
     <t>4-9</t>
+  </si>
+  <si>
+    <t>Cold tolerance - ne ako loše podnose</t>
+  </si>
+  <si>
+    <t>Heat tolerance - ne ako loše podnose</t>
+  </si>
+  <si>
+    <t>Grooming needs - da ako su zahtjevni</t>
+  </si>
+  <si>
+    <t>Protection ability - ne ako nije zaštitnički</t>
+  </si>
+  <si>
+    <t>Ease of training - ISKLJUČIVO</t>
+  </si>
+  <si>
+    <t>Friendliness toward other pets - ne ako nije prijateljski</t>
+  </si>
+  <si>
+    <t>Friendliness toward other dogs - ne ako nije prijateljski</t>
+  </si>
+  <si>
+    <t>Friendliness toward strangers - ne ako nije prijateljski</t>
+  </si>
+  <si>
+    <t>linjanje bitno - ne ako se linja</t>
   </si>
 </sst>
 </file>
@@ -489,12 +489,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -844,13 +845,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BD19" sqref="BD19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -910,175 +911,175 @@
     <row r="1" spans="1:58">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="R1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AL1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AN1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AQ1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="AS1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AY1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="BA1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AX1" s="2" t="s">
+      <c r="BC1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="AY1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>85</v>
-      </c>
       <c r="BD1" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:58">
@@ -1086,175 +1087,175 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AR2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AS2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AT2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AU2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AZ2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BA2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BC2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BF2" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:58">
@@ -1262,175 +1263,175 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AJ3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AN3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AS3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AT3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AU3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AV3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AW3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AX3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AY3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AZ3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BA3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BB3" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="BC3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BD3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BE3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BF3" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:58">
@@ -1438,175 +1439,175 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AC4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AI4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AK4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AN4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AO4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AR4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AS4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AT4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AU4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AV4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AW4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AX4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AY4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AZ4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BA4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BB4" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="BC4" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BD4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="BE4" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="BF4" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:58">
@@ -1614,1932 +1615,1761 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="X5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="Y5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AI5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AJ5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AK5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AN5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AO5" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AP5" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AR5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AS5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AT5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AU5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AV5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AW5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AX5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AY5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AZ5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BA5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BB5" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="BC5" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BD5" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BE5" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="BF5" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:58">
       <c r="A6" s="2" t="s">
-        <v>4</v>
+        <v>129</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AC6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AI6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AK6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AL6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AM6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AN6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AO6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AP6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AQ6" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AR6" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AS6" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AT6" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AU6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AV6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AW6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AX6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AY6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AZ6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BA6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BB6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="BC6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BD6" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BE6" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="BF6" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:58">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AB7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AC7" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AD7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AF7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AG7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AH7" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AI7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AK7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AL7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AM7" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AN7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AO7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AP7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AQ7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AR7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AS7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AT7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AU7" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AV7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AW7" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AX7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AY7" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AZ7" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BA7" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BB7" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BC7" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="BD7" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="BE7" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="BF7" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:58">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>130</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="Z8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AB8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AG8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AH8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AI8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AJ8" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AK8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AM8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AN8" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AO8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AP8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="AQ8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AR8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AS8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AT8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AU8" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AV8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AW8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AX8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="AY8" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="AZ8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="BA8" s="2" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="BB8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="BC8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="BD8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="BE8" s="2" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="BF8" s="3" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:58">
-      <c r="A9" s="2" t="s">
-        <v>7</v>
+      <c r="A9" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="T9" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="Z9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AB9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AG9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AH9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AI9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AJ9" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AK9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AM9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AN9" s="3" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AO9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AP9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AQ9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AR9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AS9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AT9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AU9" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AV9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AW9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="AX9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AY9" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="AZ9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BA9" s="2" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="BB9" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="BC9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BD9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BE9" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="BF9" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:58">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>126</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="T10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AB10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AG10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AH10" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="AI10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AJ10" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="AM10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AN10" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AO10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AP10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AQ10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AR10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AS10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AT10" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AU10" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="AV10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AW10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AX10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AY10" s="1" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AZ10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="BA10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="BB10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="BC10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BD10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BE10" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="BF10" s="3" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:58">
       <c r="A11" s="2" t="s">
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y11" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AB11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AC11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AG11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AH11" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AI11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AJ11" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AM11" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AN11" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AO11" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AP11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AQ11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AR11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AS11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AT11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AU11" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="AV11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="AW11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AX11" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AY11" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AZ11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="BA11" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="BB11" s="2" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="BC11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="BD11" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="BE11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="BF11" s="3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:58">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="T12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="X12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AB12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AC12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AH12" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="AI12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AJ12" s="3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="AK12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AM12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AN12" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AO12" s="2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="AP12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AQ12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AR12" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AS12" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="AT12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AU12" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="AV12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AW12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AX12" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AY12" s="1" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AZ12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="BA12" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="BB12" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="BC12" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="BD12" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="BE12" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="BF12" s="3" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:58">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="T13" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="X13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AA13" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AC13" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AG13" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="AH13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AI13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AJ13" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AK13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AM13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AN13" s="3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AO13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AP13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AQ13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AR13" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="AS13" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AT13" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="AU13" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="AV13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AW13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AX13" s="2" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="AY13" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="AZ13" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="BA13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BB13" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="BC13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="BD13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="BE13" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="BF13" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:58">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="X14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AA14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AH14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AJ14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AK14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AM14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN14" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="AO14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AP14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AR14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AS14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AT14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AU14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AV14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AW14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AX14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AY14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AZ14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="BA14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BB14" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BC14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="BD14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="BE14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="BF14" s="3" t="s">
-        <v>19</v>
+    <row r="14" spans="1:58" s="4" customFormat="1">
+      <c r="B14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="U14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="V14" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="W14" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="X14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z14" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF14" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG14" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AH14" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AI14" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AJ14" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AK14" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AL14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AM14" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AN14" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AO14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AP14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ14" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AR14" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="AS14" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AT14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV14" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY14" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AZ14" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="BA14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BB14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="BC14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="BD14" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE14" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="BF14" s="4" t="s">
+        <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:58" s="4" customFormat="1">
-      <c r="B15" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="O15" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="P15" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q15" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="R15" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="S15" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="T15" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="U15" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="V15" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="W15" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="X15" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="Y15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="Z15" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA15" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="AB15" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC15" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AD15" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE15" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="AF15" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="AG15" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="AH15" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="AI15" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ15" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AK15" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AL15" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AM15" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="AN15" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="AO15" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="AP15" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="AQ15" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="AR15" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="AS15" s="4" t="s">
+    <row r="15" spans="1:58">
+      <c r="A15" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="AT15" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AU15" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="AV15" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="AW15" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="AX15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="AY15" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="AZ15" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="BA15" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="BB15" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="BC15" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="BD15" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="BE15" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="BF15" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dodani svi psi u bazu i dodana nova pitanja
</commit_message>
<xml_diff>
--- a/pesi.xlsx
+++ b/pesi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22905"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="42220" yWindow="4760" windowWidth="25600" windowHeight="15120" tabRatio="500"/>
+    <workbookView xWindow="38400" yWindow="3440" windowWidth="33600" windowHeight="20560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,9 +402,6 @@
     <t>Protection ability - ne ako nije zaštitnički</t>
   </si>
   <si>
-    <t>Ease of training - ISKLJUČIVO</t>
-  </si>
-  <si>
     <t>Friendliness toward other pets - ne ako nije prijateljski</t>
   </si>
   <si>
@@ -415,6 +412,9 @@
   </si>
   <si>
     <t>linjanje bitno - ne ako se linja</t>
+  </si>
+  <si>
+    <t>Ease of training - da ako ga nije lako trenirati</t>
   </si>
 </sst>
 </file>
@@ -489,13 +489,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -846,70 +849,17 @@
   <dimension ref="A1:BF15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="23.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="60" customWidth="1"/>
-    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="45" max="46" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="50" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:58">
-      <c r="A1" s="2"/>
+      <c r="A1" s="5"/>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1083,7 +1033,7 @@
       </c>
     </row>
     <row r="2" spans="1:58">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1259,7 +1209,7 @@
       </c>
     </row>
     <row r="3" spans="1:58">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1435,7 +1385,7 @@
       </c>
     </row>
     <row r="4" spans="1:58">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1611,7 +1561,7 @@
       </c>
     </row>
     <row r="5" spans="1:58">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1787,8 +1737,8 @@
       </c>
     </row>
     <row r="6" spans="1:58">
-      <c r="A6" s="2" t="s">
-        <v>129</v>
+      <c r="A6" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
@@ -1963,8 +1913,8 @@
       </c>
     </row>
     <row r="7" spans="1:58">
-      <c r="A7" s="2" t="s">
-        <v>128</v>
+      <c r="A7" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -2139,8 +2089,8 @@
       </c>
     </row>
     <row r="8" spans="1:58">
-      <c r="A8" s="2" t="s">
-        <v>130</v>
+      <c r="A8" s="5" t="s">
+        <v>129</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -2315,8 +2265,8 @@
       </c>
     </row>
     <row r="9" spans="1:58">
-      <c r="A9" s="5" t="s">
-        <v>127</v>
+      <c r="A9" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
@@ -2491,7 +2441,7 @@
       </c>
     </row>
     <row r="10" spans="1:58">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>126</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -2667,7 +2617,7 @@
       </c>
     </row>
     <row r="11" spans="1:58">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>125</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -2843,7 +2793,7 @@
       </c>
     </row>
     <row r="12" spans="1:58">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>123</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -3019,7 +2969,7 @@
       </c>
     </row>
     <row r="13" spans="1:58">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -3195,6 +3145,7 @@
       </c>
     </row>
     <row r="14" spans="1:58" s="4" customFormat="1">
+      <c r="A14" s="7"/>
       <c r="B14" s="4" t="s">
         <v>83</v>
       </c>
@@ -3368,8 +3319,8 @@
       </c>
     </row>
     <row r="15" spans="1:58">
-      <c r="A15" s="2" t="s">
-        <v>131</v>
+      <c r="A15" s="5" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>